<commit_message>
Updated code and made new graphs
</commit_message>
<xml_diff>
--- a/Data_raw/Data_Reefs_Okaro.xlsx
+++ b/Data_raw/Data_Reefs_Okaro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://waikatouniversitynz-my.sharepoint.com/personal/or81_students_waikato_ac_nz/Documents/Documents/PhD/Data/5. Reefs Ōkaro/Data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="877" documentId="8_{EA738BD4-3C10-4C16-B9AA-9AC60E71F0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A80A80B5-5E0E-4948-BFF4-01EFDFB417F1}"/>
+  <xr:revisionPtr revIDLastSave="884" documentId="8_{EA738BD4-3C10-4C16-B9AA-9AC60E71F0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FAAD82C-B96B-4286-BC02-973AC3AD619A}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="5" xr2:uid="{82E70FD8-DCC2-42F4-A4AE-B2C6CA04DC23}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{82E70FD8-DCC2-42F4-A4AE-B2C6CA04DC23}"/>
   </bookViews>
   <sheets>
     <sheet name="Site_info" sheetId="9" r:id="rId1"/>
@@ -1161,7 +1161,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -8507,8 +8507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D0A5E2-6B60-4DB6-BD87-D8830AAE9368}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -8597,7 +8597,7 @@
         <v>48</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="H3" t="s">
         <v>100</v>
@@ -8639,7 +8639,7 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="H4" t="s">
         <v>97</v>
@@ -8681,7 +8681,7 @@
       </c>
       <c r="F5" s="5"/>
       <c r="G5">
-        <v>2</v>
+        <v>122</v>
       </c>
       <c r="H5" t="s">
         <v>97</v>
@@ -8723,7 +8723,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6">
-        <v>4</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -8744,7 +8744,7 @@
       </c>
       <c r="F7" s="5"/>
       <c r="G7">
-        <v>3</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -8765,7 +8765,7 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8">
-        <v>2</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -8782,7 +8782,7 @@
         <v>172</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="J9">
         <v>22.6</v>
@@ -8814,7 +8814,7 @@
         <v>172</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="J10">
         <v>22.6</v>
@@ -8846,7 +8846,7 @@
         <v>172</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>122</v>
       </c>
       <c r="J11">
         <v>22.6</v>
@@ -8874,7 +8874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD7ECAB-20FC-432A-8BE3-F53916176ADD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>